<commit_message>
implement trie + bwt changes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conor\Documents\Conor Prog\bwt-merge\bwt-merge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conor/Documents/Programming/bwt-merge/bwt-merge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59733722-7777-4D6A-B124-F7A1CD73485C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664D8AD9-8405-8D43-9157-F1F148608F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19530" yWindow="5535" windowWidth="17115" windowHeight="12270" xr2:uid="{3FF3C669-BBBF-4F59-ACDB-A4FDEB478390}"/>
+    <workbookView xWindow="12280" yWindow="5440" windowWidth="17120" windowHeight="12280" xr2:uid="{3FF3C669-BBBF-4F59-ACDB-A4FDEB478390}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>String count</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Old merge time (ms)</t>
+  </si>
+  <si>
+    <t>Rerun, with release mode</t>
   </si>
 </sst>
 </file>
@@ -116,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -156,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -262,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -404,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -412,24 +415,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C53E3D9-68EB-4B73-8D73-27B1B37ABD21}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2048</v>
       </c>
@@ -477,7 +480,7 @@
         <v>16.232421875</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8192</v>
       </c>
@@ -502,7 +505,7 @@
         <v>19.351525878906251</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32768</v>
       </c>
@@ -527,7 +530,7 @@
         <v>19.771945190429687</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>131072</v>
       </c>
@@ -552,7 +555,7 @@
         <v>19.882986450195315</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>524288</v>
       </c>
@@ -577,7 +580,7 @@
         <v>24.074066352844238</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2097152</v>
       </c>
@@ -602,7 +605,7 @@
         <v>29.607351684570315</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4194304</v>
       </c>
@@ -627,7 +630,7 @@
         <v>33.459392428398132</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7438776</v>
       </c>
@@ -650,6 +653,137 @@
       <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>34.207639926245932</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2048</v>
+      </c>
+      <c r="B14">
+        <v>10.6252</v>
+      </c>
+      <c r="C14">
+        <v>14.603300000000001</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <v>32.121400000000001</v>
+      </c>
+      <c r="C15">
+        <v>39.704000000000001</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>32768</v>
+      </c>
+      <c r="B16">
+        <v>149.14869999999999</v>
+      </c>
+      <c r="C16">
+        <v>156.85560000000001</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>131072</v>
+      </c>
+      <c r="B17">
+        <v>819.89869999999996</v>
+      </c>
+      <c r="C17">
+        <v>732.73979999999995</v>
+      </c>
+      <c r="D17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>524288</v>
+      </c>
+      <c r="B18">
+        <v>3928.2964000000002</v>
+      </c>
+      <c r="C18">
+        <v>3166.4897999999998</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2097152</v>
+      </c>
+      <c r="B19">
+        <v>20510.476299999998</v>
+      </c>
+      <c r="C19">
+        <v>13865.379300000001</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4194304</v>
+      </c>
+      <c r="B20">
+        <v>53606.484700000001</v>
+      </c>
+      <c r="C20">
+        <v>29184.9133</v>
+      </c>
+      <c r="D20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7438776</v>
+      </c>
+      <c r="B21">
+        <v>91701.114000000001</v>
+      </c>
+      <c r="C21">
+        <v>56427.221700000002</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>